<commit_message>
Refact_Controllers. About, Contacts - filled
</commit_message>
<xml_diff>
--- a/Answer_1.xlsx
+++ b/Answer_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Михаил Букачук</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Протестировать</t>
+  </si>
+  <si>
+    <t>Поменять названия методов в контроллерах</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>Убрать View и view для админки в папки admin:</t>
   </si>
 </sst>
 </file>
@@ -92,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-419]dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-419]dd/mm/yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -136,7 +151,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,24 +167,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor rgb="FFC3D69B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -227,28 +224,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -552,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D20"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,44 +594,44 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>1</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="9">
         <v>44713</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>2</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="9">
         <v>44713</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>3</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="9">
         <v>44713</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -653,30 +641,30 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="12">
         <v>4</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="9">
         <v>44713</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="12">
         <v>5</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="9">
         <v>44713</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -695,25 +683,55 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
         <v>6</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="C19" s="9">
+        <v>44714</v>
+      </c>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <v>7</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="C20" s="9">
+        <v>44714</v>
+      </c>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>